<commit_message>
added sprint review protocol #3
</commit_message>
<xml_diff>
--- a/doc/SprintReviewProtocols/Sprint_Review_Protocol#2.xlsx
+++ b/doc/SprintReviewProtocols/Sprint_Review_Protocol#2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>Sprint Review Protocol</t>
   </si>
@@ -23,30 +23,54 @@
     <t>Sprint No:</t>
   </si>
   <si>
+    <t>#2</t>
+  </si>
+  <si>
     <t>Date &amp; Time</t>
   </si>
   <si>
+    <t>25.11.2021, 16:53:00</t>
+  </si>
+  <si>
     <t>Group Number</t>
   </si>
   <si>
     <t>Participant 1</t>
   </si>
   <si>
+    <t>Stefan Düx</t>
+  </si>
+  <si>
     <t>Participant 2</t>
   </si>
   <si>
+    <t>Jessica Isabella Görög</t>
+  </si>
+  <si>
     <t>Participant 3</t>
   </si>
   <si>
+    <t>Dominic Grabner</t>
+  </si>
+  <si>
     <t>Participant 4</t>
   </si>
   <si>
+    <t>Rebekka Tscheppen</t>
+  </si>
+  <si>
     <t>Participant 5</t>
   </si>
   <si>
+    <t>Lukas Varga</t>
+  </si>
+  <si>
     <t>Mentor</t>
   </si>
   <si>
+    <t>Lukas Rohatsch</t>
+  </si>
+  <si>
     <t>List the Ids of the Requirements which are subject to the review</t>
   </si>
   <si>
@@ -78,9 +102,6 @@
   </si>
   <si>
     <t>swap PoE (malfunction)</t>
-  </si>
-  <si>
-    <t>#2</t>
   </si>
   <si>
     <t>install chosen IDE</t>
@@ -158,9 +179,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -190,6 +211,95 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -198,34 +308,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -235,74 +317,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -340,11 +354,18 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -373,19 +394,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -397,13 +448,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -415,7 +472,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -427,7 +496,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -439,13 +508,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -457,19 +532,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -481,60 +562,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -548,12 +575,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -682,15 +703,6 @@
         <color auto="1"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -705,15 +717,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -733,6 +736,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -744,6 +756,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -785,138 +806,138 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1359,8 +1380,8 @@
   <sheetPr/>
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4259259259259" defaultRowHeight="15.6"/>
@@ -1415,7 +1436,9 @@
         <v>1</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
+      <c r="C4" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -1423,10 +1446,12 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
+      <c r="C5" s="7" t="s">
+        <v>4</v>
+      </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
@@ -1434,10 +1459,12 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
+      <c r="C6" s="7">
+        <v>29</v>
+      </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -1445,10 +1472,12 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="8"/>
+      <c r="C7" s="8" t="s">
+        <v>7</v>
+      </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
@@ -1456,10 +1485,12 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="9"/>
+      <c r="C8" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
@@ -1467,10 +1498,12 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B9" s="6"/>
-      <c r="C9" s="9"/>
+      <c r="C9" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
@@ -1478,10 +1511,12 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="6" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="9"/>
+      <c r="C10" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
@@ -1489,10 +1524,12 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="6" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="10"/>
+      <c r="C11" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
@@ -1500,10 +1537,12 @@
     </row>
     <row r="12" ht="16.35" spans="1:7">
       <c r="A12" s="11" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
+      <c r="C12" s="12" t="s">
+        <v>17</v>
+      </c>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
@@ -1511,7 +1550,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="13" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -1523,36 +1562,36 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="14" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="15" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C16" s="17">
         <v>0.5</v>
@@ -1564,16 +1603,18 @@
         <f t="shared" ref="E16:E27" si="0">D16-C16</f>
         <v>0</v>
       </c>
-      <c r="F16" s="18"/>
+      <c r="F16" s="18">
+        <v>1</v>
+      </c>
       <c r="G16" s="19"/>
       <c r="H16" s="16"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="15" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C17" s="17">
         <v>0.5</v>
@@ -1585,16 +1626,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F17" s="18"/>
+      <c r="F17" s="18">
+        <v>1</v>
+      </c>
       <c r="G17" s="19"/>
       <c r="H17" s="16"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="15" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C18" s="17">
         <v>3.5</v>
@@ -1606,16 +1649,18 @@
         <f t="shared" si="0"/>
         <v>-0.5</v>
       </c>
-      <c r="F18" s="18"/>
+      <c r="F18" s="18">
+        <v>1</v>
+      </c>
       <c r="G18" s="19"/>
       <c r="H18" s="16"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="15" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C19" s="17">
         <v>1.5</v>
@@ -1627,16 +1672,18 @@
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="F19" s="18"/>
+      <c r="F19" s="18">
+        <v>1</v>
+      </c>
       <c r="G19" s="19"/>
       <c r="H19" s="16"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="15" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C20" s="17">
         <v>2</v>
@@ -1656,10 +1703,10 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="15" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C21" s="17">
         <v>0.5</v>
@@ -1671,16 +1718,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F21" s="18"/>
+      <c r="F21" s="18">
+        <v>1</v>
+      </c>
       <c r="G21" s="19"/>
       <c r="H21" s="16"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="15" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C22" s="17">
         <v>0.5</v>
@@ -1692,16 +1741,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F22" s="18"/>
+      <c r="F22" s="18">
+        <v>1</v>
+      </c>
       <c r="G22" s="19"/>
       <c r="H22" s="16"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="15" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C23" s="17">
         <v>1</v>
@@ -1713,16 +1764,18 @@
         <f t="shared" si="0"/>
         <v>-0.25</v>
       </c>
-      <c r="F23" s="18"/>
+      <c r="F23" s="18">
+        <v>1</v>
+      </c>
       <c r="G23" s="19"/>
       <c r="H23" s="16"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="15" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C24" s="17">
         <v>0.25</v>
@@ -1734,16 +1787,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F24" s="18"/>
+      <c r="F24" s="18">
+        <v>1</v>
+      </c>
       <c r="G24" s="19"/>
       <c r="H24" s="16"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="15" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C25" s="17">
         <v>2</v>
@@ -1755,16 +1810,18 @@
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="F25" s="18"/>
+      <c r="F25" s="18">
+        <v>1</v>
+      </c>
       <c r="G25" s="19"/>
       <c r="H25" s="16"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="15" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C26" s="17">
         <v>2</v>
@@ -1776,16 +1833,18 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="F26" s="18"/>
+      <c r="F26" s="18">
+        <v>1</v>
+      </c>
       <c r="G26" s="19"/>
       <c r="H26" s="16"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="15" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C27" s="17">
         <v>0.5</v>
@@ -1797,7 +1856,9 @@
         <f t="shared" si="0"/>
         <v>-0.25</v>
       </c>
-      <c r="F27" s="18"/>
+      <c r="F27" s="18">
+        <v>1</v>
+      </c>
       <c r="G27" s="19"/>
       <c r="H27" s="16"/>
     </row>
@@ -1815,7 +1876,7 @@
       </c>
       <c r="F28" s="20">
         <f>COUNT(F16:F25)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G28" s="20">
         <f>COUNT(G16:G25)</f>
@@ -1826,12 +1887,12 @@
     <row r="32" spans="1:2">
       <c r="A32" s="16"/>
       <c r="B32" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" s="1" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>